<commit_message>
+ security test cases
</commit_message>
<xml_diff>
--- a/docs/2010-08-02_Test Plan/TestCase1_10.xlsx
+++ b/docs/2010-08-02_Test Plan/TestCase1_10.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="151">
   <si>
     <t>Test #</t>
     <phoneticPr fontId="21" type="noConversion"/>
@@ -513,6 +513,106 @@
   </si>
   <si>
     <t>display "missing data" message and indicate which fields are missing. no data been updated.</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>display "access deny" message</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retest case 46 for all pages</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>enter "http://www.tigers.com/admin/users.html" into the url field without login</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Redirect to login page</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Access to web pages after login</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Redirect to userList page</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retest case 48 for all pages on the menu bar</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>click one item on the menu bar after login as an admin</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>click the "view all users" menu on the menu bar after login as an admin</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Redirect to the correspoding page</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cannot access to web pages without login</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retest case 49 by using url</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>enter the page's url into url field after login as an admin</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retest case 48 for different roles</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Redirect to the corresponding page</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retest case 49 using url for different roles</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cannot access to other roles' web page</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>enter "http://www.tigers.com/admin/users.html" into the url field after login as a contractor</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retest case 53 for different pages</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>enter a proper url into the url field without login</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>enter a proper url (other roles' pages) into the url field after login as a contractor</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retest case 54 for different roles</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>enter a proper url (other roles' pages) into the url field after login as a certain role</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>enter the page's url into url field after login as a certain role</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>click one item on the menu bar after login as a certain role</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -1090,7 +1190,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1151,6 +1251,13 @@
     <xf numFmtId="15" fontId="24" fillId="24" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1549,10 +1656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2278,7 +2385,7 @@
     </row>
     <row r="47" spans="1:5" s="20" customFormat="1" ht="23.25">
       <c r="A47" s="5">
-        <f t="shared" ref="A47:A48" si="3">A46+1</f>
+        <f t="shared" ref="A47:A58" si="3">A46+1</f>
         <v>44</v>
       </c>
       <c r="B47" s="10" t="s">
@@ -2307,6 +2414,166 @@
         <v>125</v>
       </c>
       <c r="E48" s="16"/>
+    </row>
+    <row r="49" spans="1:5" s="20" customFormat="1" ht="23.25">
+      <c r="A49" s="5">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E49" s="9"/>
+    </row>
+    <row r="50" spans="1:5" s="24" customFormat="1" ht="23.25">
+      <c r="A50" s="13">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E50" s="16"/>
+    </row>
+    <row r="51" spans="1:5" s="20" customFormat="1" ht="23.25">
+      <c r="A51" s="5">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E51" s="9"/>
+    </row>
+    <row r="52" spans="1:5" s="24" customFormat="1" ht="23.25">
+      <c r="A52" s="13">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="E52" s="16"/>
+    </row>
+    <row r="53" spans="1:5" s="20" customFormat="1" ht="23.25">
+      <c r="A53" s="5">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E53" s="9"/>
+    </row>
+    <row r="54" spans="1:5" s="24" customFormat="1" ht="23.25">
+      <c r="A54" s="13">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="E54" s="16"/>
+    </row>
+    <row r="55" spans="1:5" s="20" customFormat="1" ht="23.25">
+      <c r="A55" s="5">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E55" s="9"/>
+    </row>
+    <row r="56" spans="1:5" s="24" customFormat="1" ht="23.25">
+      <c r="A56" s="13">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="C56" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E56" s="16"/>
+    </row>
+    <row r="57" spans="1:5" s="20" customFormat="1" ht="23.25">
+      <c r="A57" s="5">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E57" s="9"/>
+    </row>
+    <row r="58" spans="1:5" s="24" customFormat="1" ht="23.25">
+      <c r="A58" s="13">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="C58" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E58" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>

</xml_diff>

<commit_message>
+ test cases for use case 10
</commit_message>
<xml_diff>
--- a/docs/2010-08-02_Test Plan/TestCase1_10.xlsx
+++ b/docs/2010-08-02_Test Plan/TestCase1_10.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="161">
   <si>
     <t>Test #</t>
     <phoneticPr fontId="21" type="noConversion"/>
@@ -520,10 +520,6 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>Retest case 46 for all pages</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <t>enter "http://www.tigers.com/admin/users.html" into the url field without login</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
@@ -540,10 +536,6 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>Retest case 48 for all pages on the menu bar</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <t>click one item on the menu bar after login as an admin</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
@@ -560,26 +552,14 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>Retest case 49 by using url</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <t>enter the page's url into url field after login as an admin</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>Retest case 48 for different roles</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <t>Redirect to the corresponding page</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>Retest case 49 using url for different roles</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <t>Cannot access to other roles' web page</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
@@ -588,10 +568,6 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>Retest case 53 for different pages</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <t>enter a proper url into the url field without login</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
@@ -600,10 +576,6 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>Retest case 54 for different roles</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <t>enter a proper url (other roles' pages) into the url field after login as a certain role</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
@@ -617,6 +589,70 @@
   </si>
   <si>
     <t>Use Case</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Upload sampler media file with incorrect file format</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Upload sampler media file with correct file format (jpg)</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Upload sampler media file with correct file format (wmv)</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>upload a media file with .jpg format</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>upload a media file with .wmv format</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>display "invalid file format" messag. No file been uploaded.</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>display "upload successfully" message. File been uploadded.</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>upload a media file with .java format</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>security</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retest case 49 for all pages</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retest case 51 for all pages on the menu bar</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retest case 52 by using url</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retest case 52 using url for different roles</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retest case 52 for different roles</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retest case 56 for different pages</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retest case 56 for different roles</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -624,7 +660,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -793,6 +829,13 @@
     <font>
       <i/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1218,7 +1261,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1304,6 +1347,23 @@
     <xf numFmtId="0" fontId="22" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="24" fillId="25" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="24" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1702,10 +1762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1718,22 +1778,22 @@
     <col min="6" max="6" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25">
+    <row r="1" spans="1:10" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="20.25">
+    <row r="2" spans="1:10" ht="20.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="25.5">
+    <row r="3" spans="1:10" ht="25.5">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>1</v>
@@ -1748,7 +1808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="23.25" customHeight="1">
+    <row r="4" spans="1:10" ht="23.25" customHeight="1">
       <c r="A4" s="12">
         <v>1</v>
       </c>
@@ -1766,7 +1826,7 @@
       </c>
       <c r="F4" s="15"/>
     </row>
-    <row r="5" spans="1:6" ht="21" customHeight="1">
+    <row r="5" spans="1:10" ht="21" customHeight="1">
       <c r="A5" s="5">
         <f>A4+1</f>
         <v>2</v>
@@ -1785,7 +1845,7 @@
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" ht="21" customHeight="1">
+    <row r="6" spans="1:10" ht="21" customHeight="1">
       <c r="A6" s="12">
         <f>A5+1</f>
         <v>3</v>
@@ -1804,7 +1864,7 @@
       </c>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1">
+    <row r="7" spans="1:10" s="18" customFormat="1" ht="21" customHeight="1">
       <c r="A7" s="5">
         <f>A6+1</f>
         <v>4</v>
@@ -1822,8 +1882,12 @@
         <v>39</v>
       </c>
       <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" ht="38.25" customHeight="1">
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+    </row>
+    <row r="8" spans="1:10" ht="38.25" customHeight="1">
       <c r="A8" s="12">
         <f t="shared" ref="A8:A34" si="0">A7+1</f>
         <v>5</v>
@@ -1842,7 +1906,7 @@
       </c>
       <c r="F8" s="16"/>
     </row>
-    <row r="9" spans="1:6" s="18" customFormat="1" ht="38.25" customHeight="1">
+    <row r="9" spans="1:10" s="18" customFormat="1" ht="38.25" customHeight="1">
       <c r="A9" s="5">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1860,8 +1924,12 @@
         <v>46</v>
       </c>
       <c r="F9" s="8"/>
-    </row>
-    <row r="10" spans="1:6" ht="23.25" customHeight="1">
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+    </row>
+    <row r="10" spans="1:10" ht="23.25" customHeight="1">
       <c r="A10" s="12">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1880,7 +1948,7 @@
       </c>
       <c r="F10" s="16"/>
     </row>
-    <row r="11" spans="1:6" s="18" customFormat="1" ht="23.25" customHeight="1">
+    <row r="11" spans="1:10" s="18" customFormat="1" ht="23.25" customHeight="1">
       <c r="A11" s="5">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1898,8 +1966,12 @@
         <v>51</v>
       </c>
       <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" ht="23.25">
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+    </row>
+    <row r="12" spans="1:10" ht="23.25">
       <c r="A12" s="12">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1918,7 +1990,7 @@
       </c>
       <c r="F12" s="16"/>
     </row>
-    <row r="13" spans="1:6" s="18" customFormat="1" ht="23.25" customHeight="1">
+    <row r="13" spans="1:10" s="18" customFormat="1" ht="23.25" customHeight="1">
       <c r="A13" s="5">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1936,8 +2008,12 @@
         <v>48</v>
       </c>
       <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" ht="33.75">
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+    </row>
+    <row r="14" spans="1:10" ht="33.75">
       <c r="A14" s="12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1956,7 +2032,7 @@
       </c>
       <c r="F14" s="16"/>
     </row>
-    <row r="15" spans="1:6" s="18" customFormat="1" ht="33.75">
+    <row r="15" spans="1:10" s="18" customFormat="1" ht="33.75">
       <c r="A15" s="5">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1974,8 +2050,12 @@
         <v>55</v>
       </c>
       <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:6" ht="33.75">
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+    </row>
+    <row r="16" spans="1:10" ht="33.75">
       <c r="A16" s="12">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1994,7 +2074,7 @@
       </c>
       <c r="F16" s="16"/>
     </row>
-    <row r="17" spans="1:6" s="18" customFormat="1" ht="33.75">
+    <row r="17" spans="1:10" s="18" customFormat="1" ht="33.75">
       <c r="A17" s="5">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2012,8 +2092,12 @@
         <v>59</v>
       </c>
       <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" ht="21" customHeight="1">
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+    </row>
+    <row r="18" spans="1:10" ht="21" customHeight="1">
       <c r="A18" s="12">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2032,7 +2116,7 @@
       </c>
       <c r="F18" s="16"/>
     </row>
-    <row r="19" spans="1:6" s="18" customFormat="1" ht="23.25">
+    <row r="19" spans="1:10" s="18" customFormat="1" ht="23.25">
       <c r="A19" s="5">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2050,8 +2134,12 @@
         <v>63</v>
       </c>
       <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" ht="33.75">
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+    </row>
+    <row r="20" spans="1:10" ht="33.75">
       <c r="A20" s="12">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2070,7 +2158,7 @@
       </c>
       <c r="F20" s="16"/>
     </row>
-    <row r="21" spans="1:6" s="18" customFormat="1" ht="33.75">
+    <row r="21" spans="1:10" s="18" customFormat="1" ht="33.75">
       <c r="A21" s="5">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2088,8 +2176,12 @@
         <v>55</v>
       </c>
       <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" ht="23.25">
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+    </row>
+    <row r="22" spans="1:10" ht="23.25">
       <c r="A22" s="12">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2108,7 +2200,7 @@
       </c>
       <c r="F22" s="16"/>
     </row>
-    <row r="23" spans="1:6" s="18" customFormat="1" ht="23.25">
+    <row r="23" spans="1:10" s="18" customFormat="1" ht="23.25">
       <c r="A23" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2126,8 +2218,12 @@
         <v>71</v>
       </c>
       <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" ht="23.25">
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+    </row>
+    <row r="24" spans="1:10" ht="23.25">
       <c r="A24" s="12">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2146,7 +2242,7 @@
       </c>
       <c r="F24" s="16"/>
     </row>
-    <row r="25" spans="1:6" s="18" customFormat="1" ht="23.25">
+    <row r="25" spans="1:10" s="18" customFormat="1" ht="23.25">
       <c r="A25" s="5">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2164,8 +2260,12 @@
         <v>73</v>
       </c>
       <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:6" ht="23.25">
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+    </row>
+    <row r="26" spans="1:10" ht="23.25">
       <c r="A26" s="12">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2184,7 +2284,7 @@
       </c>
       <c r="F26" s="16"/>
     </row>
-    <row r="27" spans="1:6" s="18" customFormat="1" ht="21" customHeight="1">
+    <row r="27" spans="1:10" s="18" customFormat="1" ht="21" customHeight="1">
       <c r="A27" s="5">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2202,8 +2302,12 @@
         <v>73</v>
       </c>
       <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:6" ht="23.25">
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+    </row>
+    <row r="28" spans="1:10" ht="23.25">
       <c r="A28" s="12">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2222,7 +2326,7 @@
       </c>
       <c r="F28" s="15"/>
     </row>
-    <row r="29" spans="1:6" s="18" customFormat="1" ht="23.25">
+    <row r="29" spans="1:10" s="18" customFormat="1" ht="23.25">
       <c r="A29" s="5">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2240,8 +2344,12 @@
         <v>73</v>
       </c>
       <c r="F29" s="9"/>
-    </row>
-    <row r="30" spans="1:6" ht="21" customHeight="1">
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+    </row>
+    <row r="30" spans="1:10" ht="21" customHeight="1">
       <c r="A30" s="12">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2260,7 +2368,7 @@
       </c>
       <c r="F30" s="15"/>
     </row>
-    <row r="31" spans="1:6" s="18" customFormat="1" ht="23.25">
+    <row r="31" spans="1:10" s="18" customFormat="1" ht="23.25">
       <c r="A31" s="5">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2278,8 +2386,12 @@
         <v>73</v>
       </c>
       <c r="F31" s="9"/>
-    </row>
-    <row r="32" spans="1:6" ht="45">
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+    </row>
+    <row r="32" spans="1:10" ht="45">
       <c r="A32" s="12">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2298,7 +2410,7 @@
       </c>
       <c r="F32" s="15"/>
     </row>
-    <row r="33" spans="1:6" s="18" customFormat="1" ht="45">
+    <row r="33" spans="1:10" s="18" customFormat="1" ht="45">
       <c r="A33" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2316,8 +2428,12 @@
         <v>95</v>
       </c>
       <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="1:6" ht="23.25">
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+    </row>
+    <row r="34" spans="1:10" ht="23.25">
       <c r="A34" s="12">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2336,7 +2452,7 @@
       </c>
       <c r="F34" s="15"/>
     </row>
-    <row r="35" spans="1:6" s="18" customFormat="1" ht="33.75">
+    <row r="35" spans="1:10" s="18" customFormat="1" ht="33.75">
       <c r="A35" s="5">
         <f t="shared" ref="A35:A39" si="1">A34+1</f>
         <v>32</v>
@@ -2354,8 +2470,12 @@
         <v>94</v>
       </c>
       <c r="F35" s="9"/>
-    </row>
-    <row r="36" spans="1:6" ht="33.75">
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+    </row>
+    <row r="36" spans="1:10" ht="33.75">
       <c r="A36" s="12">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -2374,7 +2494,7 @@
       </c>
       <c r="F36" s="15"/>
     </row>
-    <row r="37" spans="1:6" s="18" customFormat="1" ht="45">
+    <row r="37" spans="1:10" s="18" customFormat="1" ht="45">
       <c r="A37" s="5">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -2392,8 +2512,12 @@
         <v>85</v>
       </c>
       <c r="F37" s="9"/>
-    </row>
-    <row r="38" spans="1:6" ht="33.75">
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+    </row>
+    <row r="38" spans="1:10" ht="33.75">
       <c r="A38" s="12">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -2412,7 +2536,7 @@
       </c>
       <c r="F38" s="15"/>
     </row>
-    <row r="39" spans="1:6" s="18" customFormat="1" ht="33.75">
+    <row r="39" spans="1:10" s="18" customFormat="1" ht="33.75">
       <c r="A39" s="5">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -2430,8 +2554,12 @@
         <v>121</v>
       </c>
       <c r="F39" s="9"/>
-    </row>
-    <row r="40" spans="1:6" ht="33.75">
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+    </row>
+    <row r="40" spans="1:10" ht="33.75">
       <c r="A40" s="12">
         <f t="shared" ref="A40:A46" si="2">A39+1</f>
         <v>37</v>
@@ -2450,7 +2578,7 @@
       </c>
       <c r="F40" s="15"/>
     </row>
-    <row r="41" spans="1:6" s="18" customFormat="1" ht="33.75">
+    <row r="41" spans="1:10" s="18" customFormat="1" ht="33.75">
       <c r="A41" s="5">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -2468,8 +2596,12 @@
         <v>118</v>
       </c>
       <c r="F41" s="9"/>
-    </row>
-    <row r="42" spans="1:6" ht="23.25">
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+    </row>
+    <row r="42" spans="1:10" ht="23.25">
       <c r="A42" s="12">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -2488,7 +2620,7 @@
       </c>
       <c r="F42" s="15"/>
     </row>
-    <row r="43" spans="1:6" s="18" customFormat="1" ht="23.25">
+    <row r="43" spans="1:10" s="18" customFormat="1" ht="23.25">
       <c r="A43" s="5">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -2506,8 +2638,12 @@
         <v>112</v>
       </c>
       <c r="F43" s="9"/>
-    </row>
-    <row r="44" spans="1:6" ht="23.25">
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+    </row>
+    <row r="44" spans="1:10" ht="23.25">
       <c r="A44" s="24">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -2526,7 +2662,7 @@
       </c>
       <c r="F44" s="15"/>
     </row>
-    <row r="45" spans="1:6" s="18" customFormat="1" ht="23.25">
+    <row r="45" spans="1:10" s="18" customFormat="1" ht="23.25">
       <c r="A45" s="25">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -2544,8 +2680,12 @@
         <v>119</v>
       </c>
       <c r="F45" s="9"/>
-    </row>
-    <row r="46" spans="1:6" ht="33.75">
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+    </row>
+    <row r="46" spans="1:10" ht="33.75">
       <c r="A46" s="24">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -2564,9 +2704,9 @@
       </c>
       <c r="F46" s="15"/>
     </row>
-    <row r="47" spans="1:6" s="18" customFormat="1" ht="23.25">
+    <row r="47" spans="1:10" s="18" customFormat="1" ht="23.25">
       <c r="A47" s="25">
-        <f t="shared" ref="A47:A58" si="3">A46+1</f>
+        <f t="shared" ref="A47:A68" si="3">A46+1</f>
         <v>44</v>
       </c>
       <c r="B47" s="30">
@@ -2582,8 +2722,12 @@
         <v>123</v>
       </c>
       <c r="F47" s="9"/>
-    </row>
-    <row r="48" spans="1:6" ht="33.75">
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47"/>
+    </row>
+    <row r="48" spans="1:10" ht="33.75">
       <c r="A48" s="24">
         <f t="shared" si="3"/>
         <v>45</v>
@@ -2602,7 +2746,7 @@
       </c>
       <c r="F48" s="15"/>
     </row>
-    <row r="49" spans="1:6" s="18" customFormat="1" ht="23.25">
+    <row r="49" spans="1:10" s="18" customFormat="1" ht="23.25">
       <c r="A49" s="25">
         <f t="shared" si="3"/>
         <v>46</v>
@@ -2611,17 +2755,21 @@
         <v>10</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="F49" s="9"/>
-    </row>
-    <row r="50" spans="1:6" s="21" customFormat="1" ht="23.25">
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49"/>
+    </row>
+    <row r="50" spans="1:10" s="21" customFormat="1" ht="23.25">
       <c r="A50" s="24">
         <f t="shared" si="3"/>
         <v>47</v>
@@ -2629,18 +2777,22 @@
       <c r="B50" s="29">
         <v>10</v>
       </c>
-      <c r="C50" s="28" t="s">
-        <v>127</v>
+      <c r="C50" s="20" t="s">
+        <v>147</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="F50" s="15"/>
-    </row>
-    <row r="51" spans="1:6" s="18" customFormat="1" ht="23.25">
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+    </row>
+    <row r="51" spans="1:10" s="18" customFormat="1" ht="23.25">
       <c r="A51" s="25">
         <f t="shared" si="3"/>
         <v>48</v>
@@ -2648,149 +2800,246 @@
       <c r="B51" s="30">
         <v>10</v>
       </c>
-      <c r="C51" s="11" t="s">
-        <v>130</v>
+      <c r="C51" s="27" t="s">
+        <v>145</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="F51" s="9"/>
-    </row>
-    <row r="52" spans="1:6" s="21" customFormat="1" ht="23.25">
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51"/>
+    </row>
+    <row r="52" spans="1:10" s="21" customFormat="1" ht="23.25">
       <c r="A52" s="24">
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="B52" s="29">
-        <v>10</v>
+      <c r="B52" s="31" t="s">
+        <v>153</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F52" s="15"/>
-    </row>
-    <row r="53" spans="1:6" s="18" customFormat="1" ht="23.25">
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+      <c r="J52"/>
+    </row>
+    <row r="53" spans="1:10" s="18" customFormat="1" ht="23.25">
       <c r="A53" s="25">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="B53" s="30">
-        <v>10</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>138</v>
+      <c r="B53" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C53" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>139</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="F53" s="9"/>
-    </row>
-    <row r="54" spans="1:6" s="21" customFormat="1" ht="23.25">
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53"/>
+      <c r="J53"/>
+    </row>
+    <row r="54" spans="1:10" s="21" customFormat="1" ht="23.25">
       <c r="A54" s="24">
         <f t="shared" si="3"/>
         <v>51</v>
       </c>
-      <c r="B54" s="29">
-        <v>10</v>
-      </c>
-      <c r="C54" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="D54" s="20" t="s">
-        <v>150</v>
+      <c r="B54" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>132</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F54" s="15"/>
-    </row>
-    <row r="55" spans="1:6" s="18" customFormat="1" ht="23.25">
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+      <c r="J54"/>
+    </row>
+    <row r="55" spans="1:10" s="18" customFormat="1" ht="23.25">
       <c r="A55" s="25">
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
-      <c r="B55" s="30">
-        <v>10</v>
-      </c>
-      <c r="C55" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>149</v>
+      <c r="B55" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F55" s="9"/>
-    </row>
-    <row r="56" spans="1:6" s="21" customFormat="1" ht="23.25">
+      <c r="G55"/>
+      <c r="H55"/>
+      <c r="I55"/>
+      <c r="J55"/>
+    </row>
+    <row r="56" spans="1:10" s="21" customFormat="1" ht="23.25">
       <c r="A56" s="24">
         <f t="shared" si="3"/>
         <v>53</v>
       </c>
-      <c r="B56" s="29">
-        <v>10</v>
-      </c>
-      <c r="C56" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="D56" s="20" t="s">
-        <v>143</v>
+      <c r="B56" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>135</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="F56" s="15"/>
-    </row>
-    <row r="57" spans="1:6" s="18" customFormat="1" ht="23.25">
+      <c r="G56"/>
+      <c r="H56"/>
+      <c r="I56"/>
+      <c r="J56"/>
+    </row>
+    <row r="57" spans="1:10" s="18" customFormat="1" ht="23.25">
       <c r="A57" s="25">
         <f t="shared" si="3"/>
         <v>54</v>
       </c>
-      <c r="B57" s="30">
-        <v>10</v>
+      <c r="B57" s="35" t="s">
+        <v>153</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="F57" s="9"/>
-    </row>
-    <row r="58" spans="1:6" s="21" customFormat="1" ht="23.25">
+      <c r="G57"/>
+      <c r="H57"/>
+      <c r="I57"/>
+      <c r="J57"/>
+    </row>
+    <row r="58" spans="1:10" s="21" customFormat="1" ht="23.25">
       <c r="A58" s="24">
         <f t="shared" si="3"/>
         <v>55</v>
       </c>
-      <c r="B58" s="29">
-        <v>10</v>
+      <c r="B58" s="31" t="s">
+        <v>153</v>
       </c>
       <c r="C58" s="28" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E58" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="F58" s="33"/>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58"/>
+      <c r="J58"/>
+    </row>
+    <row r="59" spans="1:10" s="18" customFormat="1" ht="23.25">
+      <c r="A59" s="25">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+      <c r="B59" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C59" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E59" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="F58" s="15"/>
+      <c r="F59" s="37"/>
+      <c r="G59"/>
+      <c r="H59"/>
+      <c r="I59"/>
+      <c r="J59"/>
+    </row>
+    <row r="60" spans="1:10" ht="23.25">
+      <c r="A60" s="24">
+        <f t="shared" si="3"/>
+        <v>57</v>
+      </c>
+      <c r="B60" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="E60" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="F60" s="34"/>
+    </row>
+    <row r="61" spans="1:10" s="18" customFormat="1" ht="23.25">
+      <c r="A61" s="25">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="B61" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C61" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E61" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="F61" s="37"/>
+      <c r="G61"/>
+      <c r="H61"/>
+      <c r="I61"/>
+      <c r="J61"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>

</xml_diff>